<commit_message>
adding link to HW1
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -478,6 +478,11 @@
           <t>[Lab 0](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab0%2Flab0-rev.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[Hwk 1](https://tinyurl.com/demog180-fa23-hwk01)</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>EK Ch. 1-2</t>

</xml_diff>

<commit_message>
adding link to hw2
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -548,6 +548,11 @@
           <t>[Lab 1](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab1%2Flab_complete_network_data.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[Hwk 2](https://datahub.berkeley.edu/user/cmisunas/notebooks/demog180-fa2023/hwk/hwk02/hwk_clusteringcoef.ipynb)</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>TODO NEWSPAPER</t>

</xml_diff>

<commit_message>
adding link to lab2
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -583,6 +583,11 @@
           <t>[Triadic closure in an email network](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Ftriadic_closure%2Femail-eu-core.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[Lab 2](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab2%2Flab2_personal_networks.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>EK Ch. 3</t>

</xml_diff>

<commit_message>
adding link to demo
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -673,6 +673,11 @@
           <t>Networks in context; homophily; positive and negative networks</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[Structural balance demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Fstructural_balance%2Fstructural_balance_in_the_small_slashdot_network.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>Watts Ch. 2</t>

</xml_diff>

<commit_message>
adding links to lab3
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -638,6 +638,11 @@
           <t>[Strength of weak ties demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Fstrength_of_weak_ties%2Fsowt_wiki_talk.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[Lab 3](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab3%2Flab03_homophily.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>TODO NEWSPAPER</t>

</xml_diff>

<commit_message>
adding link to hw4
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -643,6 +643,11 @@
           <t>[Lab 3](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab3%2Flab03_homophily.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[Hwk 4](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk04%2Fhw04_balance_smallworlds.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>TODO NEWSPAPER</t>

</xml_diff>

<commit_message>
adding link to lab4
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -693,6 +693,11 @@
           <t>[Structural balance demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Fstructural_balance%2Fstructural_balance_in_the_small_slashdot_network.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[Lab 4](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab%25204%2Flab04_affiliation_networks.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>Watts Ch. 2</t>

</xml_diff>

<commit_message>
adding link to hw5
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -488,11 +488,6 @@
           <t>[Lab 0](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab0%2Flab0-rev.ipynb&amp;branch=main)</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>[Hwk 1](https://tinyurl.com/demog180-fa23-hwk01)</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>EK Ch. 1-2</t>
@@ -543,14 +538,9 @@
           <t>Personal networks; social connectedness and social isolation in America</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>[Lab 1](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab1%2Flab_complete_network_data.ipynb&amp;branch=main)</t>
-        </is>
-      </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[Hwk 2](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk02%2Fhwk_clusteringcoef.ipynb&amp;branch=main)</t>
+          <t>[Hwk 1](https://tinyurl.com/demog180-fa23-hwk01)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -585,12 +575,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[Lab 2](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab2%2Flab2_personal_networks.ipynb&amp;branch=main)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>[Hwk 3](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk03%2Fhwk03_personal_networks.ipynb&amp;branch=main)</t>
+          <t>[Lab 1](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab1%2Flab_complete_network_data.ipynb&amp;branch=main)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -638,14 +623,9 @@
           <t>[Strength of weak ties demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Fstrength_of_weak_ties%2Fsowt_wiki_talk.ipynb&amp;branch=main)</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>[Lab 3](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab3%2Flab03_homophily.ipynb&amp;branch=main)</t>
-        </is>
-      </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[Hwk 4](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk04%2Fhw04_balance_smallworlds.ipynb&amp;branch=main)</t>
+          <t>[Hwk 2](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk02%2Fhwk_clusteringcoef.ipynb&amp;branch=main)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -695,7 +675,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[Lab 4](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab%25204%2Flab04_affiliation_networks.ipynb&amp;branch=main)</t>
+          <t>[Lab 2](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab2%2Flab2_personal_networks.ipynb&amp;branch=main)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -743,6 +723,11 @@
           <t>[ER random networks demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Fer_random_networks%2Fer_random_networks.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[Hwk 3](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk03%2Fhwk03_personal_networks.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>[Triadic closure in an email network][triadic closure demo]</t>
@@ -768,6 +753,11 @@
           <t>Small worlds</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[Lab 3](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab3%2Flab03_homophily.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>EK Ch. 41-4.2; Ch. 5.1-5.2</t>
@@ -813,6 +803,11 @@
           <t>Search in small worlds</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[Hwk 4](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk04%2Fhw04_balance_smallworlds.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
           <t>Watts Ch. 3</t>
@@ -848,6 +843,11 @@
           <t>[Two mode network demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flecture%2Ftwo_mode_networks%2Ftwo_mode_networks.ipynb&amp;branch=main)</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[Lab 4](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab%25204%2Flab04_affiliation_networks.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
           <t>Watts Ch. 4</t>
@@ -896,6 +896,11 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>[netlogo ba model](https://www.netlogoweb.org/launch#https://www.netlogoweb.org/assets/modelslib/Sample%20Models/Networks/Preferential%20Attachment.nlogo)</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[Hwk 5](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk05%2Fhwk05_small_worlds.ipynb&amp;branch=main)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">

</xml_diff>

<commit_message>
adding link to lab5
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -1038,6 +1038,11 @@
           <t>Diseases and simple contagion in general; SIR model</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>[Lab 5](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Flab%2Flab5%2Flab5_centrality_sirmodel.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>Quiz 1 - [Studies of network structure](#sec:networkstructure)</t>

</xml_diff>

<commit_message>
adding link to hw7
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2023.xlsx
+++ b/syllabus/demog180 - 2023.xlsx
@@ -1303,6 +1303,11 @@
           <t>Is obesity contagious? Experimental and observational studies of complex contagion</t>
         </is>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>[Hwk 7](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2023&amp;urlpath=tree%2Fdemog180-fa2023%2Fhwk%2Fhwk07%2Fhwk07_friendship_paradox.ipynb&amp;branch=main)</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr">
         <is>
           <t>Complex contagion on networks, cont.</t>

</xml_diff>